<commit_message>
Notebook de la modelisation 2
</commit_message>
<xml_diff>
--- a/data/raw/Orano-données-Double.xlsx
+++ b/data/raw/Orano-données-Double.xlsx
@@ -321,7 +321,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="75">
   <si>
     <t>Commandes</t>
   </si>
@@ -544,6 +544,9 @@
   <si>
     <t>%</t>
   </si>
+  <si>
+    <t>Np</t>
+  </si>
 </sst>
 </file>
 
@@ -668,7 +671,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -861,13 +864,53 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -974,12 +1017,6 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1001,11 +1038,27 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="0" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="0" borderId="20" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Milliers_export-SO-2013-03-05 MOSAIC 2013" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -3670,10 +3723,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:N149"/>
+  <dimension ref="A3:O149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3692,31 +3745,31 @@
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39" t="s">
+    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="D4" s="42" t="s">
+      <c r="B4" s="38"/>
+      <c r="D4" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="39" t="s">
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
-      <c r="L4" s="42" t="s">
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="M4" s="43"/>
-      <c r="N4" s="44"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M4" s="41"/>
+      <c r="N4" s="42"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -3757,7 +3810,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>69</v>
       </c>
@@ -3794,11 +3847,14 @@
       <c r="M6" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" s="45" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>1</v>
       </c>
@@ -3839,11 +3895,14 @@
         <f ca="1">G7-L7</f>
         <v>90</v>
       </c>
-      <c r="N7" s="36">
+      <c r="N7" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" s="46">
+        <v>4.1500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>2</v>
       </c>
@@ -3883,14 +3942,17 @@
         <v>44317</v>
       </c>
       <c r="M8" s="7">
-        <f t="shared" ref="M8:M53" ca="1" si="1">G8-L8</f>
+        <f ca="1">G8-L8</f>
         <v>61</v>
       </c>
-      <c r="N8" s="36">
+      <c r="N8" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8" s="46">
+        <v>4.0999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>3</v>
       </c>
@@ -3907,18 +3969,18 @@
         <v>44199</v>
       </c>
       <c r="G9" s="10">
-        <f t="shared" ref="G9:G53" si="2">EDATE(G8,1)</f>
+        <f t="shared" ref="G9:G53" si="1">EDATE(G8,1)</f>
         <v>44409</v>
       </c>
       <c r="H9" s="14">
         <v>18.738048272122583</v>
       </c>
       <c r="I9" s="6">
-        <f t="shared" ref="I9:I53" si="3">J8</f>
+        <f t="shared" ref="I9:I53" si="2">J8</f>
         <v>44262.190782481419</v>
       </c>
       <c r="J9" s="8">
-        <f t="shared" ref="J9:J53" si="4">I9+H9</f>
+        <f>I9+H9</f>
         <v>44280.928830753539</v>
       </c>
       <c r="K9" s="9">
@@ -3930,14 +3992,17 @@
         <v>44317</v>
       </c>
       <c r="M9" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G9-L9</f>
         <v>92</v>
       </c>
-      <c r="N9" s="36">
+      <c r="N9" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" s="46">
+        <v>4.0999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>4</v>
       </c>
@@ -3954,18 +4019,18 @@
         <v>44200</v>
       </c>
       <c r="G10" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44440</v>
       </c>
       <c r="H10" s="14">
         <v>6.0447291071835094</v>
       </c>
       <c r="I10" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44280.928830753539</v>
       </c>
       <c r="J10" s="8">
-        <f t="shared" si="4"/>
+        <f>I10+H10</f>
         <v>44286.973559860722</v>
       </c>
       <c r="K10" s="9">
@@ -3977,14 +4042,17 @@
         <v>44317</v>
       </c>
       <c r="M10" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G10-L10</f>
         <v>123</v>
       </c>
-      <c r="N10" s="36">
+      <c r="N10" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" s="46">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <v>5</v>
       </c>
@@ -4001,18 +4069,18 @@
         <v>44201</v>
       </c>
       <c r="G11" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44470</v>
       </c>
       <c r="H11" s="14">
         <v>71.008938170736101</v>
       </c>
       <c r="I11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44286.973559860722</v>
       </c>
       <c r="J11" s="8">
-        <f t="shared" si="4"/>
+        <f>I11+H11</f>
         <v>44357.982498031459</v>
       </c>
       <c r="K11" s="9">
@@ -4024,14 +4092,17 @@
         <v>44408</v>
       </c>
       <c r="M11" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G11-L11</f>
         <v>62</v>
       </c>
-      <c r="N11" s="36">
+      <c r="N11" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11" s="46">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <v>6</v>
       </c>
@@ -4048,18 +4119,18 @@
         <v>44202</v>
       </c>
       <c r="G12" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44501</v>
       </c>
       <c r="H12" s="14">
         <v>19.023993354589813</v>
       </c>
       <c r="I12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44357.982498031459</v>
       </c>
       <c r="J12" s="8">
-        <f t="shared" si="4"/>
+        <f>I12+H12</f>
         <v>44377.006491386048</v>
       </c>
       <c r="K12" s="9">
@@ -4071,14 +4142,17 @@
         <v>44408</v>
       </c>
       <c r="M12" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G12-L12</f>
         <v>93</v>
       </c>
-      <c r="N12" s="36">
+      <c r="N12" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12" s="46">
+        <v>4.0999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <v>7</v>
       </c>
@@ -4095,18 +4169,18 @@
         <v>44203</v>
       </c>
       <c r="G13" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44531</v>
       </c>
       <c r="H13" s="14">
         <v>91.397392312343911</v>
       </c>
       <c r="I13" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44377.006491386048</v>
       </c>
       <c r="J13" s="8">
-        <f t="shared" si="4"/>
+        <f>I13+H13</f>
         <v>44468.403883698389</v>
       </c>
       <c r="K13" s="9">
@@ -4118,14 +4192,17 @@
         <v>44500</v>
       </c>
       <c r="M13" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G13-L13</f>
         <v>31</v>
       </c>
-      <c r="N13" s="36">
+      <c r="N13" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13" s="46">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <v>8</v>
       </c>
@@ -4142,18 +4219,18 @@
         <v>44204</v>
       </c>
       <c r="G14" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44562</v>
       </c>
       <c r="H14" s="14">
         <v>100.43780432615303</v>
       </c>
       <c r="I14" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44468.403883698389</v>
       </c>
       <c r="J14" s="8">
-        <f t="shared" si="4"/>
+        <f>I14+H14</f>
         <v>44568.841688024542</v>
       </c>
       <c r="K14" s="9">
@@ -4165,14 +4242,17 @@
         <v>44623</v>
       </c>
       <c r="M14" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G14-L14</f>
         <v>-61</v>
       </c>
-      <c r="N14" s="36">
+      <c r="N14" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" s="46">
+        <v>4.0999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>9</v>
       </c>
@@ -4189,18 +4269,18 @@
         <v>44205</v>
       </c>
       <c r="G15" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44593</v>
       </c>
       <c r="H15" s="14">
         <v>19.985794411269485</v>
       </c>
       <c r="I15" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44568.841688024542</v>
       </c>
       <c r="J15" s="8">
-        <f t="shared" si="4"/>
+        <f>I15+H15</f>
         <v>44588.827482435809</v>
       </c>
       <c r="K15" s="9">
@@ -4212,14 +4292,17 @@
         <v>44623</v>
       </c>
       <c r="M15" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G15-L15</f>
         <v>-30</v>
       </c>
-      <c r="N15" s="36">
+      <c r="N15" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" s="46">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <v>10</v>
       </c>
@@ -4236,18 +4319,18 @@
         <v>44206</v>
       </c>
       <c r="G16" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44621</v>
       </c>
       <c r="H16" s="14">
         <v>66.262665981598033</v>
       </c>
       <c r="I16" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44588.827482435809</v>
       </c>
       <c r="J16" s="8">
-        <f t="shared" si="4"/>
+        <f>I16+H16</f>
         <v>44655.09014841741</v>
       </c>
       <c r="K16" s="9">
@@ -4259,14 +4342,17 @@
         <v>44712</v>
       </c>
       <c r="M16" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G16-L16</f>
         <v>-91</v>
       </c>
-      <c r="N16" s="36">
+      <c r="N16" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" s="46">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <v>11</v>
       </c>
@@ -4283,18 +4369,18 @@
         <v>44207</v>
       </c>
       <c r="G17" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44652</v>
       </c>
       <c r="H17" s="14">
         <v>50.971380124670937</v>
       </c>
       <c r="I17" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44655.09014841741</v>
       </c>
       <c r="J17" s="8">
-        <f t="shared" si="4"/>
+        <f>I17+H17</f>
         <v>44706.061528542079</v>
       </c>
       <c r="K17" s="9">
@@ -4306,14 +4392,17 @@
         <v>44743</v>
       </c>
       <c r="M17" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G17-L17</f>
         <v>-91</v>
       </c>
-      <c r="N17" s="36">
+      <c r="N17" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17" s="46">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <v>12</v>
       </c>
@@ -4330,18 +4419,18 @@
         <v>44208</v>
       </c>
       <c r="G18" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44682</v>
       </c>
       <c r="H18" s="14">
         <v>70.966533793091116</v>
       </c>
       <c r="I18" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44706.061528542079</v>
       </c>
       <c r="J18" s="8">
-        <f t="shared" si="4"/>
+        <f>I18+H18</f>
         <v>44777.028062335172</v>
       </c>
       <c r="K18" s="9">
@@ -4353,14 +4442,17 @@
         <v>44835</v>
       </c>
       <c r="M18" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G18-L18</f>
         <v>-153</v>
       </c>
-      <c r="N18" s="36">
+      <c r="N18" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" s="46">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <v>13</v>
       </c>
@@ -4377,18 +4469,18 @@
         <v>44209</v>
       </c>
       <c r="G19" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44713</v>
       </c>
       <c r="H19" s="14">
         <v>63.581780628128165</v>
       </c>
       <c r="I19" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44777.028062335172</v>
       </c>
       <c r="J19" s="8">
-        <f t="shared" si="4"/>
+        <f>I19+H19</f>
         <v>44840.609842963298</v>
       </c>
       <c r="K19" s="9">
@@ -4400,14 +4492,17 @@
         <v>44896</v>
       </c>
       <c r="M19" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G19-L19</f>
         <v>-183</v>
       </c>
-      <c r="N19" s="36">
+      <c r="N19" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" s="46">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <v>14</v>
       </c>
@@ -4424,18 +4519,18 @@
         <v>44210</v>
       </c>
       <c r="G20" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44743</v>
       </c>
       <c r="H20" s="14">
         <v>80.619208482891608</v>
       </c>
       <c r="I20" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44840.609842963298</v>
       </c>
       <c r="J20" s="8">
-        <f t="shared" si="4"/>
+        <f>I20+H20</f>
         <v>44921.229051446193</v>
       </c>
       <c r="K20" s="9">
@@ -4447,14 +4542,17 @@
         <v>44957</v>
       </c>
       <c r="M20" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G20-L20</f>
         <v>-214</v>
       </c>
-      <c r="N20" s="36">
+      <c r="N20" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20" s="46">
+        <v>4.6500000000000007E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>15</v>
       </c>
@@ -4471,18 +4569,18 @@
         <v>44211</v>
       </c>
       <c r="G21" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44774</v>
       </c>
       <c r="H21" s="14">
         <v>5.2154307152810686</v>
       </c>
       <c r="I21" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44921.229051446193</v>
       </c>
       <c r="J21" s="8">
-        <f t="shared" si="4"/>
+        <f>I21+H21</f>
         <v>44926.444482161474</v>
       </c>
       <c r="K21" s="9">
@@ -4494,14 +4592,17 @@
         <v>44957</v>
       </c>
       <c r="M21" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G21-L21</f>
         <v>-183</v>
       </c>
-      <c r="N21" s="36">
+      <c r="N21" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21" s="46">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>16</v>
       </c>
@@ -4518,18 +4619,18 @@
         <v>44212</v>
       </c>
       <c r="G22" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44805</v>
       </c>
       <c r="H22" s="14">
         <v>99.170079072609909</v>
       </c>
       <c r="I22" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>44926.444482161474</v>
       </c>
       <c r="J22" s="8">
-        <f t="shared" si="4"/>
+        <f>I22+H22</f>
         <v>45025.614561234084</v>
       </c>
       <c r="K22" s="9">
@@ -4541,14 +4642,17 @@
         <v>45077</v>
       </c>
       <c r="M22" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G22-L22</f>
         <v>-272</v>
       </c>
-      <c r="N22" s="36">
+      <c r="N22" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22" s="46">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>17</v>
       </c>
@@ -4565,18 +4669,18 @@
         <v>44213</v>
       </c>
       <c r="G23" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44835</v>
       </c>
       <c r="H23" s="14">
         <v>62.911239470995213</v>
       </c>
       <c r="I23" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>45025.614561234084</v>
       </c>
       <c r="J23" s="8">
-        <f t="shared" si="4"/>
+        <f>I23+H23</f>
         <v>45088.52580070508</v>
       </c>
       <c r="K23" s="9">
@@ -4588,14 +4692,17 @@
         <v>45138</v>
       </c>
       <c r="M23" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G23-L23</f>
         <v>-303</v>
       </c>
-      <c r="N23" s="36">
+      <c r="N23" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23" s="46">
+        <v>4.9500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>18</v>
       </c>
@@ -4612,18 +4719,18 @@
         <v>44214</v>
       </c>
       <c r="G24" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44866</v>
       </c>
       <c r="H24" s="14">
         <v>104.91653566864618</v>
       </c>
       <c r="I24" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>45088.52580070508</v>
       </c>
       <c r="J24" s="8">
-        <f t="shared" si="4"/>
+        <f>I24+H24</f>
         <v>45193.442336373722</v>
       </c>
       <c r="K24" s="9">
@@ -4635,14 +4742,17 @@
         <v>45230</v>
       </c>
       <c r="M24" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G24-L24</f>
         <v>-364</v>
       </c>
-      <c r="N24" s="36">
+      <c r="N24" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24" s="46">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>19</v>
       </c>
@@ -4659,18 +4769,18 @@
         <v>44215</v>
       </c>
       <c r="G25" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44896</v>
       </c>
       <c r="H25" s="14">
         <v>121.41721009794317</v>
       </c>
       <c r="I25" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>45193.442336373722</v>
       </c>
       <c r="J25" s="8">
-        <f t="shared" si="4"/>
+        <f>I25+H25</f>
         <v>45314.859546471664</v>
       </c>
       <c r="K25" s="9">
@@ -4682,14 +4792,17 @@
         <v>45353</v>
       </c>
       <c r="M25" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G25-L25</f>
         <v>-457</v>
       </c>
-      <c r="N25" s="36">
+      <c r="N25" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25" s="46">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>20</v>
       </c>
@@ -4706,18 +4819,18 @@
         <v>44216</v>
       </c>
       <c r="G26" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44927</v>
       </c>
       <c r="H26" s="14">
         <v>82.03466125092784</v>
       </c>
       <c r="I26" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>45314.859546471664</v>
       </c>
       <c r="J26" s="8">
-        <f t="shared" si="4"/>
+        <f>I26+H26</f>
         <v>45396.894207722595</v>
       </c>
       <c r="K26" s="9">
@@ -4729,14 +4842,17 @@
         <v>45443</v>
       </c>
       <c r="M26" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G26-L26</f>
         <v>-516</v>
       </c>
-      <c r="N26" s="36">
+      <c r="N26" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26" s="46">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="13">
         <v>21</v>
       </c>
@@ -4753,18 +4869,18 @@
         <v>44217</v>
       </c>
       <c r="G27" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44958</v>
       </c>
       <c r="H27" s="14">
         <v>66.312142265576355</v>
       </c>
       <c r="I27" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>45396.894207722595</v>
       </c>
       <c r="J27" s="8">
-        <f t="shared" si="4"/>
+        <f>I27+H27</f>
         <v>45463.20634998817</v>
       </c>
       <c r="K27" s="9">
@@ -4776,14 +4892,17 @@
         <v>45504</v>
       </c>
       <c r="M27" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G27-L27</f>
         <v>-546</v>
       </c>
-      <c r="N27" s="36">
+      <c r="N27" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27" s="46">
+        <v>4.0999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="13">
         <v>22</v>
       </c>
@@ -4800,18 +4919,18 @@
         <v>44218</v>
       </c>
       <c r="G28" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>44986</v>
       </c>
       <c r="H28" s="14">
         <v>8.9684065688919237</v>
       </c>
       <c r="I28" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>45463.20634998817</v>
       </c>
       <c r="J28" s="8">
-        <f t="shared" si="4"/>
+        <f>I28+H28</f>
         <v>45472.174756557062</v>
       </c>
       <c r="K28" s="9">
@@ -4823,14 +4942,17 @@
         <v>45504</v>
       </c>
       <c r="M28" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G28-L28</f>
         <v>-518</v>
       </c>
-      <c r="N28" s="36">
+      <c r="N28" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28" s="46">
+        <v>4.0999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="13">
         <v>23</v>
       </c>
@@ -4847,18 +4969,18 @@
         <v>44219</v>
       </c>
       <c r="G29" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45017</v>
       </c>
       <c r="H29" s="14">
         <v>76.311738693380008</v>
       </c>
       <c r="I29" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>45472.174756557062</v>
       </c>
       <c r="J29" s="8">
-        <f t="shared" si="4"/>
+        <f>I29+H29</f>
         <v>45548.486495250443</v>
       </c>
       <c r="K29" s="9">
@@ -4870,14 +4992,17 @@
         <v>45596</v>
       </c>
       <c r="M29" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G29-L29</f>
         <v>-579</v>
       </c>
-      <c r="N29" s="36">
+      <c r="N29" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29" s="46">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="13">
         <v>24</v>
       </c>
@@ -4894,18 +5019,18 @@
         <v>44220</v>
       </c>
       <c r="G30" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45047</v>
       </c>
       <c r="H30" s="14">
         <v>62.363640902177231</v>
       </c>
       <c r="I30" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>45548.486495250443</v>
       </c>
       <c r="J30" s="8">
-        <f t="shared" si="4"/>
+        <f>I30+H30</f>
         <v>45610.850136152621</v>
       </c>
       <c r="K30" s="9">
@@ -4917,14 +5042,17 @@
         <v>45657</v>
       </c>
       <c r="M30" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G30-L30</f>
         <v>-610</v>
       </c>
-      <c r="N30" s="36">
+      <c r="N30" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30" s="46">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="13">
         <v>25</v>
       </c>
@@ -4941,18 +5069,18 @@
         <v>44221</v>
       </c>
       <c r="G31" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45078</v>
       </c>
       <c r="H31" s="14">
         <v>63.027580796781272</v>
       </c>
       <c r="I31" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>45610.850136152621</v>
       </c>
       <c r="J31" s="8">
-        <f t="shared" si="4"/>
+        <f>I31+H31</f>
         <v>45673.877716949406</v>
       </c>
       <c r="K31" s="9">
@@ -4964,14 +5092,17 @@
         <v>45719</v>
       </c>
       <c r="M31" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G31-L31</f>
         <v>-641</v>
       </c>
-      <c r="N31" s="36">
+      <c r="N31" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31" s="46">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="13">
         <v>26</v>
       </c>
@@ -4988,18 +5119,18 @@
         <v>44222</v>
       </c>
       <c r="G32" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45108</v>
       </c>
       <c r="H32" s="14">
         <v>124.57449648246569</v>
       </c>
       <c r="I32" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>45673.877716949406</v>
       </c>
       <c r="J32" s="8">
-        <f t="shared" si="4"/>
+        <f>I32+H32</f>
         <v>45798.452213431869</v>
       </c>
       <c r="K32" s="9">
@@ -5011,14 +5142,17 @@
         <v>45839</v>
       </c>
       <c r="M32" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G32-L32</f>
         <v>-731</v>
       </c>
-      <c r="N32" s="36">
+      <c r="N32" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O32" s="46">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>27</v>
       </c>
@@ -5035,18 +5169,18 @@
         <v>44223</v>
       </c>
       <c r="G33" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45139</v>
       </c>
       <c r="H33" s="14">
         <v>183.79394401524607</v>
       </c>
       <c r="I33" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>45798.452213431869</v>
       </c>
       <c r="J33" s="8">
-        <f t="shared" si="4"/>
+        <f>I33+H33</f>
         <v>45982.246157447116</v>
       </c>
       <c r="K33" s="9">
@@ -5058,14 +5192,17 @@
         <v>46022</v>
       </c>
       <c r="M33" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G33-L33</f>
         <v>-883</v>
       </c>
-      <c r="N33" s="36">
+      <c r="N33" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33" s="46">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>28</v>
       </c>
@@ -5082,18 +5219,18 @@
         <v>44224</v>
       </c>
       <c r="G34" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45170</v>
       </c>
       <c r="H34" s="14">
         <v>49.388670184363015</v>
       </c>
       <c r="I34" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>45982.246157447116</v>
       </c>
       <c r="J34" s="8">
-        <f t="shared" si="4"/>
+        <f>I34+H34</f>
         <v>46031.634827631482</v>
       </c>
       <c r="K34" s="9">
@@ -5105,14 +5242,17 @@
         <v>46084</v>
       </c>
       <c r="M34" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G34-L34</f>
         <v>-914</v>
       </c>
-      <c r="N34" s="36">
+      <c r="N34" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34" s="46">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>29</v>
       </c>
@@ -5129,18 +5269,18 @@
         <v>44225</v>
       </c>
       <c r="G35" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45200</v>
       </c>
       <c r="H35" s="14">
         <v>180.57498964499032</v>
       </c>
       <c r="I35" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>46031.634827631482</v>
       </c>
       <c r="J35" s="8">
-        <f t="shared" si="4"/>
+        <f>I35+H35</f>
         <v>46212.209817276474</v>
       </c>
       <c r="K35" s="9">
@@ -5152,14 +5292,17 @@
         <v>46265</v>
       </c>
       <c r="M35" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G35-L35</f>
         <v>-1065</v>
       </c>
-      <c r="N35" s="36">
+      <c r="N35" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O35" s="46">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>30</v>
       </c>
@@ -5176,18 +5319,18 @@
         <v>44226</v>
       </c>
       <c r="G36" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45231</v>
       </c>
       <c r="H36" s="14">
         <v>91.335183151017191</v>
       </c>
       <c r="I36" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>46212.209817276474</v>
       </c>
       <c r="J36" s="8">
-        <f t="shared" si="4"/>
+        <f>I36+H36</f>
         <v>46303.54500042749</v>
       </c>
       <c r="K36" s="9">
@@ -5199,14 +5342,17 @@
         <v>46357</v>
       </c>
       <c r="M36" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G36-L36</f>
         <v>-1126</v>
       </c>
-      <c r="N36" s="36">
+      <c r="N36" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36" s="46">
+        <v>4.6699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>31</v>
       </c>
@@ -5223,18 +5369,18 @@
         <v>44227</v>
       </c>
       <c r="G37" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45261</v>
       </c>
       <c r="H37" s="14">
         <v>7.552572845661671</v>
       </c>
       <c r="I37" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>46303.54500042749</v>
       </c>
       <c r="J37" s="8">
-        <f t="shared" si="4"/>
+        <f>I37+H37</f>
         <v>46311.097573273153</v>
       </c>
       <c r="K37" s="9">
@@ -5246,14 +5392,17 @@
         <v>46357</v>
       </c>
       <c r="M37" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G37-L37</f>
         <v>-1096</v>
       </c>
-      <c r="N37" s="36">
+      <c r="N37" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37" s="46">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>32</v>
       </c>
@@ -5270,18 +5419,18 @@
         <v>44228</v>
       </c>
       <c r="G38" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45292</v>
       </c>
       <c r="H38" s="14">
         <v>124.09825788770928</v>
       </c>
       <c r="I38" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>46311.097573273153</v>
       </c>
       <c r="J38" s="8">
-        <f t="shared" si="4"/>
+        <f>I38+H38</f>
         <v>46435.195831160861</v>
       </c>
       <c r="K38" s="9">
@@ -5293,14 +5442,17 @@
         <v>46477</v>
       </c>
       <c r="M38" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G38-L38</f>
         <v>-1185</v>
       </c>
-      <c r="N38" s="36">
+      <c r="N38" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38" s="46">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
         <v>33</v>
       </c>
@@ -5317,18 +5469,18 @@
         <v>44229</v>
       </c>
       <c r="G39" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45323</v>
       </c>
       <c r="H39" s="14">
         <v>163.82573384982302</v>
       </c>
       <c r="I39" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>46435.195831160861</v>
       </c>
       <c r="J39" s="8">
-        <f t="shared" si="4"/>
+        <f>I39+H39</f>
         <v>46599.021565010684</v>
       </c>
       <c r="K39" s="9">
@@ -5340,14 +5492,17 @@
         <v>46630</v>
       </c>
       <c r="M39" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G39-L39</f>
         <v>-1307</v>
       </c>
-      <c r="N39" s="36">
+      <c r="N39" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39" s="46">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
         <v>34</v>
       </c>
@@ -5364,18 +5519,18 @@
         <v>44230</v>
       </c>
       <c r="G40" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45352</v>
       </c>
       <c r="H40" s="14">
         <v>3.2842756186795898</v>
       </c>
       <c r="I40" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>46599.021565010684</v>
       </c>
       <c r="J40" s="8">
-        <f t="shared" si="4"/>
+        <f>I40+H40</f>
         <v>46602.305840629364</v>
       </c>
       <c r="K40" s="9">
@@ -5387,14 +5542,17 @@
         <v>46661</v>
       </c>
       <c r="M40" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G40-L40</f>
         <v>-1309</v>
       </c>
-      <c r="N40" s="36">
+      <c r="N40" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O40" s="46">
+        <v>4.0999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
         <v>35</v>
       </c>
@@ -5411,18 +5569,18 @@
         <v>44231</v>
       </c>
       <c r="G41" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45383</v>
       </c>
       <c r="H41" s="14">
         <v>2.8915996739505965</v>
       </c>
       <c r="I41" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>46602.305840629364</v>
       </c>
       <c r="J41" s="8">
-        <f t="shared" si="4"/>
+        <f>I41+H41</f>
         <v>46605.197440303316</v>
       </c>
       <c r="K41" s="9">
@@ -5434,14 +5592,17 @@
         <v>46661</v>
       </c>
       <c r="M41" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G41-L41</f>
         <v>-1278</v>
       </c>
-      <c r="N41" s="36">
+      <c r="N41" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41" s="46">
+        <v>4.4000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
         <v>36</v>
       </c>
@@ -5458,18 +5619,18 @@
         <v>44232</v>
       </c>
       <c r="G42" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45413</v>
       </c>
       <c r="H42" s="14">
         <v>103.06735426762448</v>
       </c>
       <c r="I42" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>46605.197440303316</v>
       </c>
       <c r="J42" s="8">
-        <f t="shared" si="4"/>
+        <f>I42+H42</f>
         <v>46708.26479457094</v>
       </c>
       <c r="K42" s="9">
@@ -5481,14 +5642,17 @@
         <v>46752</v>
       </c>
       <c r="M42" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G42-L42</f>
         <v>-1339</v>
       </c>
-      <c r="N42" s="36">
+      <c r="N42" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42" s="46">
+        <v>4.0999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
         <v>37</v>
       </c>
@@ -5505,18 +5669,18 @@
         <v>44233</v>
       </c>
       <c r="G43" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45444</v>
       </c>
       <c r="H43" s="14">
         <v>4.5219828676905065</v>
       </c>
       <c r="I43" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>46708.26479457094</v>
       </c>
       <c r="J43" s="8">
-        <f t="shared" si="4"/>
+        <f>I43+H43</f>
         <v>46712.786777438632</v>
       </c>
       <c r="K43" s="9">
@@ -5528,14 +5692,17 @@
         <v>46752</v>
       </c>
       <c r="M43" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G43-L43</f>
         <v>-1308</v>
       </c>
-      <c r="N43" s="36">
+      <c r="N43" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43" s="46">
+        <v>4.0999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>38</v>
       </c>
@@ -5552,18 +5719,18 @@
         <v>44234</v>
       </c>
       <c r="G44" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45474</v>
       </c>
       <c r="H44" s="14">
         <v>61.580011888955248</v>
       </c>
       <c r="I44" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>46712.786777438632</v>
       </c>
       <c r="J44" s="8">
-        <f t="shared" si="4"/>
+        <f>I44+H44</f>
         <v>46774.366789327585</v>
       </c>
       <c r="K44" s="9">
@@ -5575,14 +5742,17 @@
         <v>46814</v>
       </c>
       <c r="M44" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G44-L44</f>
         <v>-1340</v>
       </c>
-      <c r="N44" s="36">
+      <c r="N44" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O44" s="46">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="13">
         <v>39</v>
       </c>
@@ -5599,18 +5769,18 @@
         <v>44235</v>
       </c>
       <c r="G45" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45505</v>
       </c>
       <c r="H45" s="14">
         <v>41.950542433683758</v>
       </c>
       <c r="I45" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>46774.366789327585</v>
       </c>
       <c r="J45" s="8">
-        <f t="shared" si="4"/>
+        <f>I45+H45</f>
         <v>46816.317331761267</v>
       </c>
       <c r="K45" s="9">
@@ -5622,14 +5792,17 @@
         <v>46874</v>
       </c>
       <c r="M45" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G45-L45</f>
         <v>-1369</v>
       </c>
-      <c r="N45" s="36">
+      <c r="N45" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O45" s="46">
+        <v>4.3700000000000003E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
         <v>40</v>
       </c>
@@ -5646,18 +5819,18 @@
         <v>44236</v>
       </c>
       <c r="G46" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45536</v>
       </c>
       <c r="H46" s="14">
         <v>25.261514611808177</v>
       </c>
       <c r="I46" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>46816.317331761267</v>
       </c>
       <c r="J46" s="8">
-        <f t="shared" si="4"/>
+        <f>I46+H46</f>
         <v>46841.578846373079</v>
       </c>
       <c r="K46" s="9">
@@ -5669,14 +5842,17 @@
         <v>46874</v>
       </c>
       <c r="M46" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G46-L46</f>
         <v>-1338</v>
       </c>
-      <c r="N46" s="36">
+      <c r="N46" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O46" s="46">
+        <v>4.0999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
         <v>41</v>
       </c>
@@ -5693,18 +5869,18 @@
         <v>44237</v>
       </c>
       <c r="G47" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45566</v>
       </c>
       <c r="H47" s="14">
         <v>71.609672947864183</v>
       </c>
       <c r="I47" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>46841.578846373079</v>
       </c>
       <c r="J47" s="8">
-        <f t="shared" si="4"/>
+        <f>I47+H47</f>
         <v>46913.188519320945</v>
       </c>
       <c r="K47" s="9">
@@ -5716,14 +5892,17 @@
         <v>46965</v>
       </c>
       <c r="M47" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G47-L47</f>
         <v>-1399</v>
       </c>
-      <c r="N47" s="36">
+      <c r="N47" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O47" s="46">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
         <v>42</v>
       </c>
@@ -5740,18 +5919,18 @@
         <v>44238</v>
       </c>
       <c r="G48" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45597</v>
       </c>
       <c r="H48" s="14">
         <v>15.425560686366785</v>
       </c>
       <c r="I48" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>46913.188519320945</v>
       </c>
       <c r="J48" s="8">
-        <f t="shared" si="4"/>
+        <f>I48+H48</f>
         <v>46928.614080007312</v>
       </c>
       <c r="K48" s="9">
@@ -5763,14 +5942,17 @@
         <v>46965</v>
       </c>
       <c r="M48" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G48-L48</f>
         <v>-1368</v>
       </c>
-      <c r="N48" s="36">
+      <c r="N48" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O48" s="46">
+        <v>4.4000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="13">
         <v>43</v>
       </c>
@@ -5787,18 +5969,18 @@
         <v>44239</v>
       </c>
       <c r="G49" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45627</v>
       </c>
       <c r="H49" s="14">
         <v>7.9176558365248804</v>
       </c>
       <c r="I49" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>46928.614080007312</v>
       </c>
       <c r="J49" s="8">
-        <f t="shared" si="4"/>
+        <f>I49+H49</f>
         <v>46936.531735843833</v>
       </c>
       <c r="K49" s="9">
@@ -5810,14 +5992,17 @@
         <v>46996</v>
       </c>
       <c r="M49" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G49-L49</f>
         <v>-1369</v>
       </c>
-      <c r="N49" s="36">
+      <c r="N49" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O49" s="46">
+        <v>4.0999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="13">
         <v>44</v>
       </c>
@@ -5834,18 +6019,18 @@
         <v>44240</v>
       </c>
       <c r="G50" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45658</v>
       </c>
       <c r="H50" s="14">
         <v>23.890602133078644</v>
       </c>
       <c r="I50" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>46936.531735843833</v>
       </c>
       <c r="J50" s="8">
-        <f t="shared" si="4"/>
+        <f>I50+H50</f>
         <v>46960.42233797691</v>
       </c>
       <c r="K50" s="9">
@@ -5857,14 +6042,17 @@
         <v>46996</v>
       </c>
       <c r="M50" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G50-L50</f>
         <v>-1338</v>
       </c>
-      <c r="N50" s="36">
+      <c r="N50" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O50" s="46">
+        <v>4.0999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="13">
         <v>45</v>
       </c>
@@ -5881,18 +6069,18 @@
         <v>44241</v>
       </c>
       <c r="G51" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45689</v>
       </c>
       <c r="H51" s="14">
         <v>2.9309573532106676</v>
       </c>
       <c r="I51" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>46960.42233797691</v>
       </c>
       <c r="J51" s="8">
-        <f t="shared" si="4"/>
+        <f>I51+H51</f>
         <v>46963.353295330118</v>
       </c>
       <c r="K51" s="9">
@@ -5904,14 +6092,17 @@
         <v>46996</v>
       </c>
       <c r="M51" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G51-L51</f>
         <v>-1307</v>
       </c>
-      <c r="N51" s="36">
+      <c r="N51" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O51" s="46">
+        <v>4.0999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="13">
         <v>46</v>
       </c>
@@ -5928,18 +6119,18 @@
         <v>44242</v>
       </c>
       <c r="G52" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45717</v>
       </c>
       <c r="H52" s="14">
         <v>89.581861417052849</v>
       </c>
       <c r="I52" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>46963.353295330118</v>
       </c>
       <c r="J52" s="8">
-        <f t="shared" si="4"/>
+        <f>I52+H52</f>
         <v>47052.935156747168</v>
       </c>
       <c r="K52" s="9">
@@ -5951,14 +6142,17 @@
         <v>47088</v>
       </c>
       <c r="M52" s="7">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G52-L52</f>
         <v>-1371</v>
       </c>
-      <c r="N52" s="36">
+      <c r="N52" s="43">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O52" s="46">
+        <v>4.4000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="13">
         <v>47</v>
       </c>
@@ -5975,18 +6169,18 @@
         <v>44243</v>
       </c>
       <c r="G53" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>45748</v>
       </c>
       <c r="H53" s="16">
         <v>21.10197024477165</v>
       </c>
       <c r="I53" s="30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>47052.935156747168</v>
       </c>
       <c r="J53" s="31">
-        <f t="shared" si="4"/>
+        <f>I53+H53</f>
         <v>47074.037126991941</v>
       </c>
       <c r="K53" s="32">
@@ -5998,26 +6192,29 @@
         <v>47118</v>
       </c>
       <c r="M53" s="35">
-        <f t="shared" ca="1" si="1"/>
+        <f ca="1">G53-L53</f>
         <v>-1370</v>
       </c>
-      <c r="N53" s="37">
+      <c r="N53" s="44">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O53" s="47">
+        <v>4.4000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="13">
         <v>48</v>
       </c>
       <c r="B54" s="28">
         <v>45627</v>
       </c>
-      <c r="H54" s="38">
+      <c r="H54" s="36">
         <f>AVERAGE(H7:H53)</f>
         <v>61.213555893445672</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="13">
         <v>49</v>
       </c>
@@ -6025,7 +6222,7 @@
         <v>45658</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="13">
         <v>50</v>
       </c>
@@ -6033,7 +6230,7 @@
         <v>45689</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="13">
         <v>51</v>
       </c>
@@ -6041,7 +6238,7 @@
         <v>45717</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="13">
         <v>52</v>
       </c>
@@ -6049,7 +6246,7 @@
         <v>45748</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="13">
         <v>53</v>
       </c>
@@ -6057,7 +6254,7 @@
         <v>45778</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="13">
         <v>54</v>
       </c>
@@ -6065,7 +6262,7 @@
         <v>45809</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="13">
         <v>55</v>
       </c>
@@ -6073,7 +6270,7 @@
         <v>45839</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="13">
         <v>56</v>
       </c>
@@ -6081,7 +6278,7 @@
         <v>45870</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="13">
         <v>57</v>
       </c>
@@ -6089,7 +6286,7 @@
         <v>45901</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="13">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
Mise à jour modèle 2
</commit_message>
<xml_diff>
--- a/data/raw/Orano-données-Double.xlsx
+++ b/data/raw/Orano-données-Double.xlsx
@@ -1020,6 +1020,21 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="0" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="0" borderId="20" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1037,21 +1052,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="20" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3725,8 +3725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3747,27 +3747,27 @@
   <sheetData>
     <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="D4" s="40" t="s">
+      <c r="B4" s="43"/>
+      <c r="D4" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="37" t="s">
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="40" t="s">
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="M4" s="41"/>
-      <c r="N4" s="42"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="47"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -3850,7 +3850,7 @@
       <c r="N6" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="O6" s="45" t="s">
+      <c r="O6" s="39" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3880,7 +3880,7 @@
         <v>44197</v>
       </c>
       <c r="J7" s="10">
-        <f>I7+H7</f>
+        <f t="shared" ref="J7:J53" si="0">I7+H7</f>
         <v>44203.057056413818</v>
       </c>
       <c r="K7" s="9">
@@ -3892,13 +3892,13 @@
         <v>44258</v>
       </c>
       <c r="M7" s="7">
-        <f ca="1">G7-L7</f>
+        <f t="shared" ref="M7:M53" ca="1" si="1">G7-L7</f>
         <v>90</v>
       </c>
-      <c r="N7" s="43">
+      <c r="N7" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O7" s="46">
+      <c r="O7" s="40">
         <v>4.1500000000000002E-2</v>
       </c>
     </row>
@@ -3930,11 +3930,11 @@
         <v>44203.057056413818</v>
       </c>
       <c r="J8" s="8">
-        <f>I8+H8</f>
+        <f t="shared" si="0"/>
         <v>44262.190782481419</v>
       </c>
       <c r="K8" s="9">
-        <f t="shared" ref="K8:K53" ca="1" si="0">OFFSET($B$6,1+MATCH(J8,$B$7:$B$150,1),0)</f>
+        <f t="shared" ref="K8:K53" ca="1" si="2">OFFSET($B$6,1+MATCH(J8,$B$7:$B$150,1),0)</f>
         <v>44287</v>
       </c>
       <c r="L8" s="33">
@@ -3942,13 +3942,13 @@
         <v>44317</v>
       </c>
       <c r="M8" s="7">
-        <f ca="1">G8-L8</f>
+        <f t="shared" ca="1" si="1"/>
         <v>61</v>
       </c>
-      <c r="N8" s="43">
+      <c r="N8" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O8" s="46">
+      <c r="O8" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
     </row>
@@ -3969,22 +3969,22 @@
         <v>44199</v>
       </c>
       <c r="G9" s="10">
-        <f t="shared" ref="G9:G53" si="1">EDATE(G8,1)</f>
+        <f t="shared" ref="G9:G53" si="3">EDATE(G8,1)</f>
         <v>44409</v>
       </c>
       <c r="H9" s="14">
         <v>18.738048272122583</v>
       </c>
       <c r="I9" s="6">
-        <f t="shared" ref="I9:I53" si="2">J8</f>
+        <f t="shared" ref="I9:I53" si="4">J8</f>
         <v>44262.190782481419</v>
       </c>
       <c r="J9" s="8">
-        <f>I9+H9</f>
+        <f t="shared" si="0"/>
         <v>44280.928830753539</v>
       </c>
       <c r="K9" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>44287</v>
       </c>
       <c r="L9" s="33">
@@ -3992,13 +3992,13 @@
         <v>44317</v>
       </c>
       <c r="M9" s="7">
-        <f ca="1">G9-L9</f>
+        <f t="shared" ca="1" si="1"/>
         <v>92</v>
       </c>
-      <c r="N9" s="43">
+      <c r="N9" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O9" s="46">
+      <c r="O9" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
     </row>
@@ -4019,22 +4019,22 @@
         <v>44200</v>
       </c>
       <c r="G10" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44440</v>
       </c>
       <c r="H10" s="14">
         <v>6.0447291071835094</v>
       </c>
       <c r="I10" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44280.928830753539</v>
       </c>
       <c r="J10" s="8">
-        <f>I10+H10</f>
+        <f t="shared" si="0"/>
         <v>44286.973559860722</v>
       </c>
       <c r="K10" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>44287</v>
       </c>
       <c r="L10" s="33">
@@ -4042,13 +4042,13 @@
         <v>44317</v>
       </c>
       <c r="M10" s="7">
-        <f ca="1">G10-L10</f>
+        <f t="shared" ca="1" si="1"/>
         <v>123</v>
       </c>
-      <c r="N10" s="43">
+      <c r="N10" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O10" s="46">
+      <c r="O10" s="40">
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
@@ -4069,22 +4069,22 @@
         <v>44201</v>
       </c>
       <c r="G11" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44470</v>
       </c>
       <c r="H11" s="14">
         <v>71.008938170736101</v>
       </c>
       <c r="I11" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44286.973559860722</v>
       </c>
       <c r="J11" s="8">
-        <f>I11+H11</f>
+        <f t="shared" si="0"/>
         <v>44357.982498031459</v>
       </c>
       <c r="K11" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>44378</v>
       </c>
       <c r="L11" s="33">
@@ -4092,13 +4092,13 @@
         <v>44408</v>
       </c>
       <c r="M11" s="7">
-        <f ca="1">G11-L11</f>
+        <f t="shared" ca="1" si="1"/>
         <v>62</v>
       </c>
-      <c r="N11" s="43">
+      <c r="N11" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O11" s="46">
+      <c r="O11" s="40">
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
@@ -4119,22 +4119,22 @@
         <v>44202</v>
       </c>
       <c r="G12" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44501</v>
       </c>
       <c r="H12" s="14">
         <v>19.023993354589813</v>
       </c>
       <c r="I12" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44357.982498031459</v>
       </c>
       <c r="J12" s="8">
-        <f>I12+H12</f>
+        <f t="shared" si="0"/>
         <v>44377.006491386048</v>
       </c>
       <c r="K12" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>44378</v>
       </c>
       <c r="L12" s="33">
@@ -4142,13 +4142,13 @@
         <v>44408</v>
       </c>
       <c r="M12" s="7">
-        <f ca="1">G12-L12</f>
+        <f t="shared" ca="1" si="1"/>
         <v>93</v>
       </c>
-      <c r="N12" s="43">
+      <c r="N12" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O12" s="46">
+      <c r="O12" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
     </row>
@@ -4169,22 +4169,22 @@
         <v>44203</v>
       </c>
       <c r="G13" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44531</v>
       </c>
       <c r="H13" s="14">
         <v>91.397392312343911</v>
       </c>
       <c r="I13" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44377.006491386048</v>
       </c>
       <c r="J13" s="8">
-        <f>I13+H13</f>
+        <f t="shared" si="0"/>
         <v>44468.403883698389</v>
       </c>
       <c r="K13" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>44470</v>
       </c>
       <c r="L13" s="33">
@@ -4192,13 +4192,13 @@
         <v>44500</v>
       </c>
       <c r="M13" s="7">
-        <f ca="1">G13-L13</f>
+        <f t="shared" ca="1" si="1"/>
         <v>31</v>
       </c>
-      <c r="N13" s="43">
+      <c r="N13" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O13" s="46">
+      <c r="O13" s="40">
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
@@ -4219,22 +4219,22 @@
         <v>44204</v>
       </c>
       <c r="G14" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44562</v>
       </c>
       <c r="H14" s="14">
         <v>100.43780432615303</v>
       </c>
       <c r="I14" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44468.403883698389</v>
       </c>
       <c r="J14" s="8">
-        <f>I14+H14</f>
+        <f t="shared" si="0"/>
         <v>44568.841688024542</v>
       </c>
       <c r="K14" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>44593</v>
       </c>
       <c r="L14" s="33">
@@ -4242,13 +4242,13 @@
         <v>44623</v>
       </c>
       <c r="M14" s="7">
-        <f ca="1">G14-L14</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-61</v>
       </c>
-      <c r="N14" s="43">
+      <c r="N14" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O14" s="46">
+      <c r="O14" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
     </row>
@@ -4269,22 +4269,22 @@
         <v>44205</v>
       </c>
       <c r="G15" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44593</v>
       </c>
       <c r="H15" s="14">
         <v>19.985794411269485</v>
       </c>
       <c r="I15" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44568.841688024542</v>
       </c>
       <c r="J15" s="8">
-        <f>I15+H15</f>
+        <f t="shared" si="0"/>
         <v>44588.827482435809</v>
       </c>
       <c r="K15" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>44593</v>
       </c>
       <c r="L15" s="33">
@@ -4292,13 +4292,13 @@
         <v>44623</v>
       </c>
       <c r="M15" s="7">
-        <f ca="1">G15-L15</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-30</v>
       </c>
-      <c r="N15" s="43">
+      <c r="N15" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O15" s="46">
+      <c r="O15" s="40">
         <v>0.04</v>
       </c>
     </row>
@@ -4319,22 +4319,22 @@
         <v>44206</v>
       </c>
       <c r="G16" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44621</v>
       </c>
       <c r="H16" s="14">
         <v>66.262665981598033</v>
       </c>
       <c r="I16" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44588.827482435809</v>
       </c>
       <c r="J16" s="8">
-        <f>I16+H16</f>
+        <f t="shared" si="0"/>
         <v>44655.09014841741</v>
       </c>
       <c r="K16" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>44682</v>
       </c>
       <c r="L16" s="33">
@@ -4342,13 +4342,13 @@
         <v>44712</v>
       </c>
       <c r="M16" s="7">
-        <f ca="1">G16-L16</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-91</v>
       </c>
-      <c r="N16" s="43">
+      <c r="N16" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O16" s="46">
+      <c r="O16" s="40">
         <v>0.04</v>
       </c>
     </row>
@@ -4369,22 +4369,22 @@
         <v>44207</v>
       </c>
       <c r="G17" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44652</v>
       </c>
       <c r="H17" s="14">
         <v>50.971380124670937</v>
       </c>
       <c r="I17" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44655.09014841741</v>
       </c>
       <c r="J17" s="8">
-        <f>I17+H17</f>
+        <f t="shared" si="0"/>
         <v>44706.061528542079</v>
       </c>
       <c r="K17" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>44713</v>
       </c>
       <c r="L17" s="33">
@@ -4392,13 +4392,13 @@
         <v>44743</v>
       </c>
       <c r="M17" s="7">
-        <f ca="1">G17-L17</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-91</v>
       </c>
-      <c r="N17" s="43">
+      <c r="N17" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O17" s="46">
+      <c r="O17" s="40">
         <v>0.04</v>
       </c>
     </row>
@@ -4419,22 +4419,22 @@
         <v>44208</v>
       </c>
       <c r="G18" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44682</v>
       </c>
       <c r="H18" s="14">
         <v>70.966533793091116</v>
       </c>
       <c r="I18" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44706.061528542079</v>
       </c>
       <c r="J18" s="8">
-        <f>I18+H18</f>
+        <f t="shared" si="0"/>
         <v>44777.028062335172</v>
       </c>
       <c r="K18" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>44805</v>
       </c>
       <c r="L18" s="33">
@@ -4442,13 +4442,13 @@
         <v>44835</v>
       </c>
       <c r="M18" s="7">
-        <f ca="1">G18-L18</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-153</v>
       </c>
-      <c r="N18" s="43">
+      <c r="N18" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O18" s="46">
+      <c r="O18" s="40">
         <v>0.04</v>
       </c>
     </row>
@@ -4469,22 +4469,22 @@
         <v>44209</v>
       </c>
       <c r="G19" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44713</v>
       </c>
       <c r="H19" s="14">
         <v>63.581780628128165</v>
       </c>
       <c r="I19" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44777.028062335172</v>
       </c>
       <c r="J19" s="8">
-        <f>I19+H19</f>
+        <f t="shared" si="0"/>
         <v>44840.609842963298</v>
       </c>
       <c r="K19" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>44866</v>
       </c>
       <c r="L19" s="33">
@@ -4492,13 +4492,13 @@
         <v>44896</v>
       </c>
       <c r="M19" s="7">
-        <f ca="1">G19-L19</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-183</v>
       </c>
-      <c r="N19" s="43">
+      <c r="N19" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O19" s="46">
+      <c r="O19" s="40">
         <v>0.04</v>
       </c>
     </row>
@@ -4519,22 +4519,22 @@
         <v>44210</v>
       </c>
       <c r="G20" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44743</v>
       </c>
       <c r="H20" s="14">
         <v>80.619208482891608</v>
       </c>
       <c r="I20" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44840.609842963298</v>
       </c>
       <c r="J20" s="8">
-        <f>I20+H20</f>
+        <f t="shared" si="0"/>
         <v>44921.229051446193</v>
       </c>
       <c r="K20" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>44927</v>
       </c>
       <c r="L20" s="33">
@@ -4542,13 +4542,13 @@
         <v>44957</v>
       </c>
       <c r="M20" s="7">
-        <f ca="1">G20-L20</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-214</v>
       </c>
-      <c r="N20" s="43">
+      <c r="N20" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O20" s="46">
+      <c r="O20" s="40">
         <v>4.6500000000000007E-2</v>
       </c>
     </row>
@@ -4569,22 +4569,22 @@
         <v>44211</v>
       </c>
       <c r="G21" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44774</v>
       </c>
       <c r="H21" s="14">
         <v>5.2154307152810686</v>
       </c>
       <c r="I21" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44921.229051446193</v>
       </c>
       <c r="J21" s="8">
-        <f>I21+H21</f>
+        <f t="shared" si="0"/>
         <v>44926.444482161474</v>
       </c>
       <c r="K21" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>44927</v>
       </c>
       <c r="L21" s="33">
@@ -4592,13 +4592,13 @@
         <v>44957</v>
       </c>
       <c r="M21" s="7">
-        <f ca="1">G21-L21</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-183</v>
       </c>
-      <c r="N21" s="43">
+      <c r="N21" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O21" s="46">
+      <c r="O21" s="40">
         <v>0.04</v>
       </c>
     </row>
@@ -4619,22 +4619,22 @@
         <v>44212</v>
       </c>
       <c r="G22" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44805</v>
       </c>
       <c r="H22" s="14">
         <v>99.170079072609909</v>
       </c>
       <c r="I22" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>44926.444482161474</v>
       </c>
       <c r="J22" s="8">
-        <f>I22+H22</f>
+        <f t="shared" si="0"/>
         <v>45025.614561234084</v>
       </c>
       <c r="K22" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>45047</v>
       </c>
       <c r="L22" s="33">
@@ -4642,13 +4642,13 @@
         <v>45077</v>
       </c>
       <c r="M22" s="7">
-        <f ca="1">G22-L22</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-272</v>
       </c>
-      <c r="N22" s="43">
+      <c r="N22" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O22" s="46">
+      <c r="O22" s="40">
         <v>0.04</v>
       </c>
     </row>
@@ -4669,22 +4669,22 @@
         <v>44213</v>
       </c>
       <c r="G23" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44835</v>
       </c>
       <c r="H23" s="14">
         <v>62.911239470995213</v>
       </c>
       <c r="I23" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45025.614561234084</v>
       </c>
       <c r="J23" s="8">
-        <f>I23+H23</f>
+        <f t="shared" si="0"/>
         <v>45088.52580070508</v>
       </c>
       <c r="K23" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>45108</v>
       </c>
       <c r="L23" s="33">
@@ -4692,13 +4692,13 @@
         <v>45138</v>
       </c>
       <c r="M23" s="7">
-        <f ca="1">G23-L23</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-303</v>
       </c>
-      <c r="N23" s="43">
+      <c r="N23" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O23" s="46">
+      <c r="O23" s="40">
         <v>4.9500000000000002E-2</v>
       </c>
     </row>
@@ -4719,22 +4719,22 @@
         <v>44214</v>
       </c>
       <c r="G24" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44866</v>
       </c>
       <c r="H24" s="14">
         <v>104.91653566864618</v>
       </c>
       <c r="I24" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45088.52580070508</v>
       </c>
       <c r="J24" s="8">
-        <f>I24+H24</f>
+        <f t="shared" si="0"/>
         <v>45193.442336373722</v>
       </c>
       <c r="K24" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>45200</v>
       </c>
       <c r="L24" s="33">
@@ -4742,13 +4742,13 @@
         <v>45230</v>
       </c>
       <c r="M24" s="7">
-        <f ca="1">G24-L24</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-364</v>
       </c>
-      <c r="N24" s="43">
+      <c r="N24" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O24" s="46">
+      <c r="O24" s="40">
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
@@ -4769,22 +4769,22 @@
         <v>44215</v>
       </c>
       <c r="G25" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44896</v>
       </c>
       <c r="H25" s="14">
         <v>121.41721009794317</v>
       </c>
       <c r="I25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45193.442336373722</v>
       </c>
       <c r="J25" s="8">
-        <f>I25+H25</f>
+        <f t="shared" si="0"/>
         <v>45314.859546471664</v>
       </c>
       <c r="K25" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>45323</v>
       </c>
       <c r="L25" s="33">
@@ -4792,13 +4792,13 @@
         <v>45353</v>
       </c>
       <c r="M25" s="7">
-        <f ca="1">G25-L25</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-457</v>
       </c>
-      <c r="N25" s="43">
+      <c r="N25" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O25" s="46">
+      <c r="O25" s="40">
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
@@ -4819,22 +4819,22 @@
         <v>44216</v>
       </c>
       <c r="G26" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44927</v>
       </c>
       <c r="H26" s="14">
         <v>82.03466125092784</v>
       </c>
       <c r="I26" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45314.859546471664</v>
       </c>
       <c r="J26" s="8">
-        <f>I26+H26</f>
+        <f t="shared" si="0"/>
         <v>45396.894207722595</v>
       </c>
       <c r="K26" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>45413</v>
       </c>
       <c r="L26" s="33">
@@ -4842,13 +4842,13 @@
         <v>45443</v>
       </c>
       <c r="M26" s="7">
-        <f ca="1">G26-L26</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-516</v>
       </c>
-      <c r="N26" s="43">
+      <c r="N26" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O26" s="46">
+      <c r="O26" s="40">
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
@@ -4869,22 +4869,22 @@
         <v>44217</v>
       </c>
       <c r="G27" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44958</v>
       </c>
       <c r="H27" s="14">
         <v>66.312142265576355</v>
       </c>
       <c r="I27" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45396.894207722595</v>
       </c>
       <c r="J27" s="8">
-        <f>I27+H27</f>
+        <f t="shared" si="0"/>
         <v>45463.20634998817</v>
       </c>
       <c r="K27" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>45474</v>
       </c>
       <c r="L27" s="33">
@@ -4892,13 +4892,13 @@
         <v>45504</v>
       </c>
       <c r="M27" s="7">
-        <f ca="1">G27-L27</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-546</v>
       </c>
-      <c r="N27" s="43">
+      <c r="N27" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O27" s="46">
+      <c r="O27" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
     </row>
@@ -4919,22 +4919,22 @@
         <v>44218</v>
       </c>
       <c r="G28" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>44986</v>
       </c>
       <c r="H28" s="14">
         <v>8.9684065688919237</v>
       </c>
       <c r="I28" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45463.20634998817</v>
       </c>
       <c r="J28" s="8">
-        <f>I28+H28</f>
+        <f t="shared" si="0"/>
         <v>45472.174756557062</v>
       </c>
       <c r="K28" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>45474</v>
       </c>
       <c r="L28" s="33">
@@ -4942,13 +4942,13 @@
         <v>45504</v>
       </c>
       <c r="M28" s="7">
-        <f ca="1">G28-L28</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-518</v>
       </c>
-      <c r="N28" s="43">
+      <c r="N28" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O28" s="46">
+      <c r="O28" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
     </row>
@@ -4969,22 +4969,22 @@
         <v>44219</v>
       </c>
       <c r="G29" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45017</v>
       </c>
       <c r="H29" s="14">
         <v>76.311738693380008</v>
       </c>
       <c r="I29" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45472.174756557062</v>
       </c>
       <c r="J29" s="8">
-        <f>I29+H29</f>
+        <f t="shared" si="0"/>
         <v>45548.486495250443</v>
       </c>
       <c r="K29" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>45566</v>
       </c>
       <c r="L29" s="33">
@@ -4992,13 +4992,13 @@
         <v>45596</v>
       </c>
       <c r="M29" s="7">
-        <f ca="1">G29-L29</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-579</v>
       </c>
-      <c r="N29" s="43">
+      <c r="N29" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O29" s="46">
+      <c r="O29" s="40">
         <v>0.04</v>
       </c>
     </row>
@@ -5019,22 +5019,22 @@
         <v>44220</v>
       </c>
       <c r="G30" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45047</v>
       </c>
       <c r="H30" s="14">
         <v>62.363640902177231</v>
       </c>
       <c r="I30" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45548.486495250443</v>
       </c>
       <c r="J30" s="8">
-        <f>I30+H30</f>
+        <f t="shared" si="0"/>
         <v>45610.850136152621</v>
       </c>
       <c r="K30" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>45627</v>
       </c>
       <c r="L30" s="33">
@@ -5042,13 +5042,13 @@
         <v>45657</v>
       </c>
       <c r="M30" s="7">
-        <f ca="1">G30-L30</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-610</v>
       </c>
-      <c r="N30" s="43">
+      <c r="N30" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O30" s="46">
+      <c r="O30" s="40">
         <v>0.04</v>
       </c>
     </row>
@@ -5069,22 +5069,22 @@
         <v>44221</v>
       </c>
       <c r="G31" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45078</v>
       </c>
       <c r="H31" s="14">
         <v>63.027580796781272</v>
       </c>
       <c r="I31" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45610.850136152621</v>
       </c>
       <c r="J31" s="8">
-        <f>I31+H31</f>
+        <f t="shared" si="0"/>
         <v>45673.877716949406</v>
       </c>
       <c r="K31" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>45689</v>
       </c>
       <c r="L31" s="33">
@@ -5092,13 +5092,13 @@
         <v>45719</v>
       </c>
       <c r="M31" s="7">
-        <f ca="1">G31-L31</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-641</v>
       </c>
-      <c r="N31" s="43">
+      <c r="N31" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O31" s="46">
+      <c r="O31" s="40">
         <v>0.04</v>
       </c>
     </row>
@@ -5119,22 +5119,22 @@
         <v>44222</v>
       </c>
       <c r="G32" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45108</v>
       </c>
       <c r="H32" s="14">
         <v>124.57449648246569</v>
       </c>
       <c r="I32" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45673.877716949406</v>
       </c>
       <c r="J32" s="8">
-        <f>I32+H32</f>
+        <f t="shared" si="0"/>
         <v>45798.452213431869</v>
       </c>
       <c r="K32" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>45809</v>
       </c>
       <c r="L32" s="33">
@@ -5142,13 +5142,13 @@
         <v>45839</v>
       </c>
       <c r="M32" s="7">
-        <f ca="1">G32-L32</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-731</v>
       </c>
-      <c r="N32" s="43">
+      <c r="N32" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O32" s="46">
+      <c r="O32" s="40">
         <v>0.04</v>
       </c>
     </row>
@@ -5169,22 +5169,22 @@
         <v>44223</v>
       </c>
       <c r="G33" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45139</v>
       </c>
       <c r="H33" s="14">
         <v>183.79394401524607</v>
       </c>
       <c r="I33" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45798.452213431869</v>
       </c>
       <c r="J33" s="8">
-        <f>I33+H33</f>
+        <f t="shared" si="0"/>
         <v>45982.246157447116</v>
       </c>
       <c r="K33" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>45992</v>
       </c>
       <c r="L33" s="33">
@@ -5192,13 +5192,13 @@
         <v>46022</v>
       </c>
       <c r="M33" s="7">
-        <f ca="1">G33-L33</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-883</v>
       </c>
-      <c r="N33" s="43">
+      <c r="N33" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O33" s="46">
+      <c r="O33" s="40">
         <v>0.04</v>
       </c>
     </row>
@@ -5219,22 +5219,22 @@
         <v>44224</v>
       </c>
       <c r="G34" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45170</v>
       </c>
       <c r="H34" s="14">
         <v>49.388670184363015</v>
       </c>
       <c r="I34" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45982.246157447116</v>
       </c>
       <c r="J34" s="8">
-        <f>I34+H34</f>
+        <f t="shared" si="0"/>
         <v>46031.634827631482</v>
       </c>
       <c r="K34" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>46054</v>
       </c>
       <c r="L34" s="33">
@@ -5242,13 +5242,13 @@
         <v>46084</v>
       </c>
       <c r="M34" s="7">
-        <f ca="1">G34-L34</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-914</v>
       </c>
-      <c r="N34" s="43">
+      <c r="N34" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O34" s="46">
+      <c r="O34" s="40">
         <v>0.04</v>
       </c>
     </row>
@@ -5269,22 +5269,22 @@
         <v>44225</v>
       </c>
       <c r="G35" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45200</v>
       </c>
       <c r="H35" s="14">
         <v>180.57498964499032</v>
       </c>
       <c r="I35" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>46031.634827631482</v>
       </c>
       <c r="J35" s="8">
-        <f>I35+H35</f>
+        <f t="shared" si="0"/>
         <v>46212.209817276474</v>
       </c>
       <c r="K35" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>46235</v>
       </c>
       <c r="L35" s="33">
@@ -5292,13 +5292,13 @@
         <v>46265</v>
       </c>
       <c r="M35" s="7">
-        <f ca="1">G35-L35</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-1065</v>
       </c>
-      <c r="N35" s="43">
+      <c r="N35" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O35" s="46">
+      <c r="O35" s="40">
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
@@ -5319,22 +5319,22 @@
         <v>44226</v>
       </c>
       <c r="G36" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45231</v>
       </c>
       <c r="H36" s="14">
         <v>91.335183151017191</v>
       </c>
       <c r="I36" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>46212.209817276474</v>
       </c>
       <c r="J36" s="8">
-        <f>I36+H36</f>
+        <f t="shared" si="0"/>
         <v>46303.54500042749</v>
       </c>
       <c r="K36" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>46327</v>
       </c>
       <c r="L36" s="33">
@@ -5342,13 +5342,13 @@
         <v>46357</v>
       </c>
       <c r="M36" s="7">
-        <f ca="1">G36-L36</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-1126</v>
       </c>
-      <c r="N36" s="43">
+      <c r="N36" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O36" s="46">
+      <c r="O36" s="40">
         <v>4.6699999999999998E-2</v>
       </c>
     </row>
@@ -5369,22 +5369,22 @@
         <v>44227</v>
       </c>
       <c r="G37" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45261</v>
       </c>
       <c r="H37" s="14">
         <v>7.552572845661671</v>
       </c>
       <c r="I37" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>46303.54500042749</v>
       </c>
       <c r="J37" s="8">
-        <f>I37+H37</f>
+        <f t="shared" si="0"/>
         <v>46311.097573273153</v>
       </c>
       <c r="K37" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>46327</v>
       </c>
       <c r="L37" s="33">
@@ -5392,13 +5392,13 @@
         <v>46357</v>
       </c>
       <c r="M37" s="7">
-        <f ca="1">G37-L37</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-1096</v>
       </c>
-      <c r="N37" s="43">
+      <c r="N37" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O37" s="46">
+      <c r="O37" s="40">
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
@@ -5419,22 +5419,22 @@
         <v>44228</v>
       </c>
       <c r="G38" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45292</v>
       </c>
       <c r="H38" s="14">
         <v>124.09825788770928</v>
       </c>
       <c r="I38" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>46311.097573273153</v>
       </c>
       <c r="J38" s="8">
-        <f>I38+H38</f>
+        <f t="shared" si="0"/>
         <v>46435.195831160861</v>
       </c>
       <c r="K38" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>46447</v>
       </c>
       <c r="L38" s="33">
@@ -5442,13 +5442,13 @@
         <v>46477</v>
       </c>
       <c r="M38" s="7">
-        <f ca="1">G38-L38</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-1185</v>
       </c>
-      <c r="N38" s="43">
+      <c r="N38" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O38" s="46">
+      <c r="O38" s="40">
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
@@ -5469,22 +5469,22 @@
         <v>44229</v>
       </c>
       <c r="G39" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45323</v>
       </c>
       <c r="H39" s="14">
         <v>163.82573384982302</v>
       </c>
       <c r="I39" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>46435.195831160861</v>
       </c>
       <c r="J39" s="8">
-        <f>I39+H39</f>
+        <f t="shared" si="0"/>
         <v>46599.021565010684</v>
       </c>
       <c r="K39" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>46600</v>
       </c>
       <c r="L39" s="33">
@@ -5492,13 +5492,13 @@
         <v>46630</v>
       </c>
       <c r="M39" s="7">
-        <f ca="1">G39-L39</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-1307</v>
       </c>
-      <c r="N39" s="43">
+      <c r="N39" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O39" s="46">
+      <c r="O39" s="40">
         <v>0.04</v>
       </c>
     </row>
@@ -5519,22 +5519,22 @@
         <v>44230</v>
       </c>
       <c r="G40" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45352</v>
       </c>
       <c r="H40" s="14">
         <v>3.2842756186795898</v>
       </c>
       <c r="I40" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>46599.021565010684</v>
       </c>
       <c r="J40" s="8">
-        <f>I40+H40</f>
+        <f t="shared" si="0"/>
         <v>46602.305840629364</v>
       </c>
       <c r="K40" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>46631</v>
       </c>
       <c r="L40" s="33">
@@ -5542,13 +5542,13 @@
         <v>46661</v>
       </c>
       <c r="M40" s="7">
-        <f ca="1">G40-L40</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-1309</v>
       </c>
-      <c r="N40" s="43">
+      <c r="N40" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O40" s="46">
+      <c r="O40" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
     </row>
@@ -5569,22 +5569,22 @@
         <v>44231</v>
       </c>
       <c r="G41" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45383</v>
       </c>
       <c r="H41" s="14">
         <v>2.8915996739505965</v>
       </c>
       <c r="I41" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>46602.305840629364</v>
       </c>
       <c r="J41" s="8">
-        <f>I41+H41</f>
+        <f t="shared" si="0"/>
         <v>46605.197440303316</v>
       </c>
       <c r="K41" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>46631</v>
       </c>
       <c r="L41" s="33">
@@ -5592,13 +5592,13 @@
         <v>46661</v>
       </c>
       <c r="M41" s="7">
-        <f ca="1">G41-L41</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-1278</v>
       </c>
-      <c r="N41" s="43">
+      <c r="N41" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O41" s="46">
+      <c r="O41" s="40">
         <v>4.4000000000000004E-2</v>
       </c>
     </row>
@@ -5619,22 +5619,22 @@
         <v>44232</v>
       </c>
       <c r="G42" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45413</v>
       </c>
       <c r="H42" s="14">
         <v>103.06735426762448</v>
       </c>
       <c r="I42" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>46605.197440303316</v>
       </c>
       <c r="J42" s="8">
-        <f>I42+H42</f>
+        <f t="shared" si="0"/>
         <v>46708.26479457094</v>
       </c>
       <c r="K42" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>46722</v>
       </c>
       <c r="L42" s="33">
@@ -5642,13 +5642,13 @@
         <v>46752</v>
       </c>
       <c r="M42" s="7">
-        <f ca="1">G42-L42</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-1339</v>
       </c>
-      <c r="N42" s="43">
+      <c r="N42" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O42" s="46">
+      <c r="O42" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
     </row>
@@ -5669,22 +5669,22 @@
         <v>44233</v>
       </c>
       <c r="G43" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45444</v>
       </c>
       <c r="H43" s="14">
         <v>4.5219828676905065</v>
       </c>
       <c r="I43" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>46708.26479457094</v>
       </c>
       <c r="J43" s="8">
-        <f>I43+H43</f>
+        <f t="shared" si="0"/>
         <v>46712.786777438632</v>
       </c>
       <c r="K43" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>46722</v>
       </c>
       <c r="L43" s="33">
@@ -5692,13 +5692,13 @@
         <v>46752</v>
       </c>
       <c r="M43" s="7">
-        <f ca="1">G43-L43</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-1308</v>
       </c>
-      <c r="N43" s="43">
+      <c r="N43" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O43" s="46">
+      <c r="O43" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
     </row>
@@ -5719,22 +5719,22 @@
         <v>44234</v>
       </c>
       <c r="G44" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45474</v>
       </c>
       <c r="H44" s="14">
         <v>61.580011888955248</v>
       </c>
       <c r="I44" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>46712.786777438632</v>
       </c>
       <c r="J44" s="8">
-        <f>I44+H44</f>
+        <f t="shared" si="0"/>
         <v>46774.366789327585</v>
       </c>
       <c r="K44" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>46784</v>
       </c>
       <c r="L44" s="33">
@@ -5742,13 +5742,13 @@
         <v>46814</v>
       </c>
       <c r="M44" s="7">
-        <f ca="1">G44-L44</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-1340</v>
       </c>
-      <c r="N44" s="43">
+      <c r="N44" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O44" s="46">
+      <c r="O44" s="40">
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
@@ -5769,22 +5769,22 @@
         <v>44235</v>
       </c>
       <c r="G45" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45505</v>
       </c>
       <c r="H45" s="14">
         <v>41.950542433683758</v>
       </c>
       <c r="I45" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>46774.366789327585</v>
       </c>
       <c r="J45" s="8">
-        <f>I45+H45</f>
+        <f t="shared" si="0"/>
         <v>46816.317331761267</v>
       </c>
       <c r="K45" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>46844</v>
       </c>
       <c r="L45" s="33">
@@ -5792,13 +5792,13 @@
         <v>46874</v>
       </c>
       <c r="M45" s="7">
-        <f ca="1">G45-L45</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-1369</v>
       </c>
-      <c r="N45" s="43">
+      <c r="N45" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O45" s="46">
+      <c r="O45" s="40">
         <v>4.3700000000000003E-2</v>
       </c>
     </row>
@@ -5819,22 +5819,22 @@
         <v>44236</v>
       </c>
       <c r="G46" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45536</v>
       </c>
       <c r="H46" s="14">
         <v>25.261514611808177</v>
       </c>
       <c r="I46" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>46816.317331761267</v>
       </c>
       <c r="J46" s="8">
-        <f>I46+H46</f>
+        <f t="shared" si="0"/>
         <v>46841.578846373079</v>
       </c>
       <c r="K46" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>46844</v>
       </c>
       <c r="L46" s="33">
@@ -5842,13 +5842,13 @@
         <v>46874</v>
       </c>
       <c r="M46" s="7">
-        <f ca="1">G46-L46</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-1338</v>
       </c>
-      <c r="N46" s="43">
+      <c r="N46" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O46" s="46">
+      <c r="O46" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
     </row>
@@ -5869,22 +5869,22 @@
         <v>44237</v>
       </c>
       <c r="G47" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45566</v>
       </c>
       <c r="H47" s="14">
         <v>71.609672947864183</v>
       </c>
       <c r="I47" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>46841.578846373079</v>
       </c>
       <c r="J47" s="8">
-        <f>I47+H47</f>
+        <f t="shared" si="0"/>
         <v>46913.188519320945</v>
       </c>
       <c r="K47" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>46935</v>
       </c>
       <c r="L47" s="33">
@@ -5892,13 +5892,13 @@
         <v>46965</v>
       </c>
       <c r="M47" s="7">
-        <f ca="1">G47-L47</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-1399</v>
       </c>
-      <c r="N47" s="43">
+      <c r="N47" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O47" s="46">
+      <c r="O47" s="40">
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
@@ -5919,22 +5919,22 @@
         <v>44238</v>
       </c>
       <c r="G48" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45597</v>
       </c>
       <c r="H48" s="14">
         <v>15.425560686366785</v>
       </c>
       <c r="I48" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>46913.188519320945</v>
       </c>
       <c r="J48" s="8">
-        <f>I48+H48</f>
+        <f t="shared" si="0"/>
         <v>46928.614080007312</v>
       </c>
       <c r="K48" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>46935</v>
       </c>
       <c r="L48" s="33">
@@ -5942,13 +5942,13 @@
         <v>46965</v>
       </c>
       <c r="M48" s="7">
-        <f ca="1">G48-L48</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-1368</v>
       </c>
-      <c r="N48" s="43">
+      <c r="N48" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O48" s="46">
+      <c r="O48" s="40">
         <v>4.4000000000000004E-2</v>
       </c>
     </row>
@@ -5969,22 +5969,22 @@
         <v>44239</v>
       </c>
       <c r="G49" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45627</v>
       </c>
       <c r="H49" s="14">
         <v>7.9176558365248804</v>
       </c>
       <c r="I49" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>46928.614080007312</v>
       </c>
       <c r="J49" s="8">
-        <f>I49+H49</f>
+        <f t="shared" si="0"/>
         <v>46936.531735843833</v>
       </c>
       <c r="K49" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>46966</v>
       </c>
       <c r="L49" s="33">
@@ -5992,13 +5992,13 @@
         <v>46996</v>
       </c>
       <c r="M49" s="7">
-        <f ca="1">G49-L49</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-1369</v>
       </c>
-      <c r="N49" s="43">
+      <c r="N49" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O49" s="46">
+      <c r="O49" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
     </row>
@@ -6019,22 +6019,22 @@
         <v>44240</v>
       </c>
       <c r="G50" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45658</v>
       </c>
       <c r="H50" s="14">
         <v>23.890602133078644</v>
       </c>
       <c r="I50" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>46936.531735843833</v>
       </c>
       <c r="J50" s="8">
-        <f>I50+H50</f>
+        <f t="shared" si="0"/>
         <v>46960.42233797691</v>
       </c>
       <c r="K50" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>46966</v>
       </c>
       <c r="L50" s="33">
@@ -6042,13 +6042,13 @@
         <v>46996</v>
       </c>
       <c r="M50" s="7">
-        <f ca="1">G50-L50</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-1338</v>
       </c>
-      <c r="N50" s="43">
+      <c r="N50" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O50" s="46">
+      <c r="O50" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
     </row>
@@ -6069,22 +6069,22 @@
         <v>44241</v>
       </c>
       <c r="G51" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45689</v>
       </c>
       <c r="H51" s="14">
         <v>2.9309573532106676</v>
       </c>
       <c r="I51" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>46960.42233797691</v>
       </c>
       <c r="J51" s="8">
-        <f>I51+H51</f>
+        <f t="shared" si="0"/>
         <v>46963.353295330118</v>
       </c>
       <c r="K51" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>46966</v>
       </c>
       <c r="L51" s="33">
@@ -6092,13 +6092,13 @@
         <v>46996</v>
       </c>
       <c r="M51" s="7">
-        <f ca="1">G51-L51</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-1307</v>
       </c>
-      <c r="N51" s="43">
+      <c r="N51" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O51" s="46">
+      <c r="O51" s="40">
         <v>4.0999999999999995E-2</v>
       </c>
     </row>
@@ -6119,22 +6119,22 @@
         <v>44242</v>
       </c>
       <c r="G52" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45717</v>
       </c>
       <c r="H52" s="14">
         <v>89.581861417052849</v>
       </c>
       <c r="I52" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>46963.353295330118</v>
       </c>
       <c r="J52" s="8">
-        <f>I52+H52</f>
+        <f t="shared" si="0"/>
         <v>47052.935156747168</v>
       </c>
       <c r="K52" s="9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>47058</v>
       </c>
       <c r="L52" s="33">
@@ -6142,13 +6142,13 @@
         <v>47088</v>
       </c>
       <c r="M52" s="7">
-        <f ca="1">G52-L52</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-1371</v>
       </c>
-      <c r="N52" s="43">
+      <c r="N52" s="37">
         <v>1E-3</v>
       </c>
-      <c r="O52" s="46">
+      <c r="O52" s="40">
         <v>4.4000000000000004E-2</v>
       </c>
     </row>
@@ -6169,22 +6169,22 @@
         <v>44243</v>
       </c>
       <c r="G53" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>45748</v>
       </c>
       <c r="H53" s="16">
         <v>21.10197024477165</v>
       </c>
       <c r="I53" s="30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>47052.935156747168</v>
       </c>
       <c r="J53" s="31">
-        <f>I53+H53</f>
+        <f t="shared" si="0"/>
         <v>47074.037126991941</v>
       </c>
       <c r="K53" s="32">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>47088</v>
       </c>
       <c r="L53" s="34">
@@ -6192,13 +6192,13 @@
         <v>47118</v>
       </c>
       <c r="M53" s="35">
-        <f ca="1">G53-L53</f>
+        <f t="shared" ca="1" si="1"/>
         <v>-1370</v>
       </c>
-      <c r="N53" s="44">
+      <c r="N53" s="38">
         <v>1E-3</v>
       </c>
-      <c r="O53" s="47">
+      <c r="O53" s="41">
         <v>4.4000000000000004E-2</v>
       </c>
     </row>

</xml_diff>